<commit_message>
commit up vercel test
</commit_message>
<xml_diff>
--- a/BC79-Template_Task-Nhom5.xlsx
+++ b/BC79-Template_Task-Nhom5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\Capstone-ReactJS_Nhom5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D52A06E-5EE9-4276-A454-6834DD3ED4FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA25C3F-5B45-49E0-A5C0-B6401FA015FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{0A11CD3D-94C1-44E9-8D78-103A12258948}"/>
   </bookViews>
@@ -34,17 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
   <si>
     <t>Tasks Name</t>
-  </si>
-  <si>
-    <t>Start
-Build</t>
-  </si>
-  <si>
-    <t>Finish
-Build</t>
   </si>
   <si>
     <t>% 
@@ -130,9 +122,6 @@
   </si>
   <si>
     <t>Hiển thị thông tin doanh nghiệp</t>
-  </si>
-  <si>
-    <t>Popup Login</t>
   </si>
   <si>
     <t>Đăng nhập với danh sách api
@@ -190,6 +179,9 @@
   </si>
   <si>
     <t>Trung Sơn</t>
+  </si>
+  <si>
+    <t>Link Login</t>
   </si>
 </sst>
 </file>
@@ -199,7 +191,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -320,8 +312,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="22">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -354,18 +353,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
-        <bgColor rgb="FFE2EFD9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor rgb="FFE2EFD9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor rgb="FFE2EFD9"/>
       </patternFill>
@@ -380,18 +367,6 @@
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor rgb="FFDFE3E8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -426,18 +401,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -764,63 +727,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="11" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="12" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="13" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="7" fillId="9" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -835,52 +768,22 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="16" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="7" fillId="12" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="11" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="12" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="16" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="11" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="12" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="16" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="7" fillId="12" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="12" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -892,41 +795,20 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="11" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="12" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="16" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="12" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -937,6 +819,33 @@
     <xf numFmtId="164" fontId="3" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="3" fillId="4" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -946,22 +855,43 @@
     <xf numFmtId="164" fontId="3" fillId="4" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="18" fillId="9" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1279,568 +1209,512 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{259D3F96-3246-4986-8E83-22F4B6F2EB88}">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.265625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="18" style="9" customWidth="1"/>
-    <col min="3" max="4" width="9.06640625" style="9"/>
-    <col min="5" max="5" width="18.1328125" style="9" customWidth="1"/>
-    <col min="6" max="6" width="9.06640625" style="48"/>
-    <col min="7" max="7" width="9.06640625" style="49"/>
-    <col min="8" max="8" width="9.06640625" style="50"/>
-    <col min="9" max="9" width="15.796875" style="66" customWidth="1"/>
-    <col min="10" max="10" width="9.06640625" style="51"/>
-    <col min="11" max="16384" width="9.06640625" style="9"/>
+    <col min="1" max="1" width="26.265625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="18" style="4" customWidth="1"/>
+    <col min="3" max="4" width="9.06640625" style="4"/>
+    <col min="5" max="5" width="18.1328125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="9.06640625" style="26"/>
+    <col min="7" max="7" width="15.796875" style="36" customWidth="1"/>
+    <col min="8" max="8" width="9.06640625" style="27"/>
+    <col min="9" max="16384" width="9.06640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+    </row>
+    <row r="3" spans="1:11" s="6" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="30"/>
+    </row>
+    <row r="4" spans="1:11" s="6" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5" t="s">
+      <c r="B4" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="55">
         <v>1</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="61" t="s">
+      <c r="G4" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5" spans="1:11" s="6" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="1:11" s="6" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" spans="1:11" s="6" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="1:11" s="6" customFormat="1" ht="41.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="1:11" s="6" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="9"/>
+      <c r="K9" s="10"/>
+    </row>
+    <row r="10" spans="1:11" s="6" customFormat="1" ht="19.5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="7"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="9"/>
+    </row>
+    <row r="11" spans="1:11" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+    </row>
+    <row r="12" spans="1:11" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="9"/>
+    </row>
+    <row r="13" spans="1:11" s="6" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="A13" s="50"/>
+      <c r="B13" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="9"/>
+    </row>
+    <row r="14" spans="1:11" s="6" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="A14" s="50"/>
+      <c r="B14" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" s="9"/>
+    </row>
+    <row r="15" spans="1:11" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+    </row>
+    <row r="16" spans="1:11" s="6" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="A16" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" spans="1:8" s="6" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="A17" s="50"/>
+      <c r="B17" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="9"/>
+    </row>
+    <row r="18" spans="1:8" s="6" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="A18" s="50"/>
+      <c r="B18" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" s="9"/>
+    </row>
+    <row r="19" spans="1:8" s="6" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="A19" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="51"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" s="9"/>
+    </row>
+    <row r="20" spans="1:8" s="6" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="A20" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="B20" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="H20" s="17"/>
+    </row>
+    <row r="21" spans="1:8" s="6" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="A21" s="44"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="46"/>
+    </row>
+    <row r="22" spans="1:8" ht="17.25" x14ac:dyDescent="0.45">
+      <c r="A22" s="28" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-    </row>
-    <row r="3" spans="1:13" s="13" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="58" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="62" t="s">
+      <c r="B22" s="47"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22" s="19"/>
+    </row>
+    <row r="23" spans="1:8" ht="34.5" x14ac:dyDescent="0.45">
+      <c r="A23" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="47"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" s="24"/>
+    </row>
+    <row r="24" spans="1:8" s="6" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="A24" s="44"/>
+      <c r="B24" s="45"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="46"/>
+    </row>
+    <row r="25" spans="1:8" ht="18.75" x14ac:dyDescent="0.45">
+      <c r="A25" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+    </row>
+    <row r="26" spans="1:8" s="6" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="A26" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+    </row>
+    <row r="27" spans="1:8" s="6" customFormat="1" ht="52.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="9"/>
+    </row>
+    <row r="28" spans="1:8" ht="17.649999999999999" x14ac:dyDescent="0.45">
+      <c r="A28" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="24"/>
+    </row>
+    <row r="29" spans="1:8" ht="17.649999999999999" x14ac:dyDescent="0.45">
+      <c r="A29" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="57"/>
-    </row>
-    <row r="4" spans="1:13" s="13" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="63" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" s="19"/>
-    </row>
-    <row r="5" spans="1:13" s="13" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A5" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="63" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5" s="19"/>
-    </row>
-    <row r="6" spans="1:13" s="13" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A6" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="63" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6" s="19"/>
-    </row>
-    <row r="7" spans="1:13" s="13" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A7" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="63" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" s="19"/>
-    </row>
-    <row r="8" spans="1:13" s="13" customFormat="1" ht="41.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="63" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="19"/>
-    </row>
-    <row r="9" spans="1:13" s="13" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="63" t="s">
-        <v>9</v>
-      </c>
-      <c r="J9" s="19"/>
-      <c r="M9" s="20"/>
-    </row>
-    <row r="10" spans="1:13" s="13" customFormat="1" ht="19.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="14"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="64"/>
-      <c r="J10" s="19"/>
-    </row>
-    <row r="11" spans="1:13" s="13" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-    </row>
-    <row r="12" spans="1:13" s="13" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="63" t="s">
-        <v>9</v>
-      </c>
-      <c r="J12" s="19"/>
-    </row>
-    <row r="13" spans="1:13" s="13" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A13" s="24"/>
-      <c r="B13" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="63" t="s">
-        <v>9</v>
-      </c>
-      <c r="J13" s="19"/>
-    </row>
-    <row r="14" spans="1:13" s="13" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A14" s="24"/>
-      <c r="B14" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="63" t="s">
-        <v>9</v>
-      </c>
-      <c r="J14" s="19"/>
-    </row>
-    <row r="15" spans="1:13" s="13" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-    </row>
-    <row r="16" spans="1:13" s="13" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A16" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="J16" s="19"/>
-    </row>
-    <row r="17" spans="1:10" s="13" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A17" s="24"/>
-      <c r="B17" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="J17" s="19"/>
-    </row>
-    <row r="18" spans="1:10" s="13" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A18" s="24"/>
-      <c r="B18" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="J18" s="19"/>
-    </row>
-    <row r="19" spans="1:10" s="13" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A19" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="J19" s="19"/>
-    </row>
-    <row r="20" spans="1:10" s="13" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A20" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="J20" s="32"/>
-    </row>
-    <row r="21" spans="1:10" s="13" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A21" s="33"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="35"/>
-    </row>
-    <row r="22" spans="1:10" ht="17.25" x14ac:dyDescent="0.45">
-      <c r="A22" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="52"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="54"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="63" t="s">
-        <v>9</v>
-      </c>
-      <c r="J22" s="39"/>
-    </row>
-    <row r="23" spans="1:10" ht="34.5" x14ac:dyDescent="0.45">
-      <c r="A23" s="56" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="52"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="63" t="s">
-        <v>9</v>
-      </c>
-      <c r="J23" s="46"/>
-    </row>
-    <row r="24" spans="1:10" s="13" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A24" s="33"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="35"/>
-    </row>
-    <row r="25" spans="1:10" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="A25" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-    </row>
-    <row r="26" spans="1:10" s="13" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A26" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-    </row>
-    <row r="27" spans="1:10" s="13" customFormat="1" ht="52.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="64"/>
-      <c r="J27" s="19"/>
-    </row>
-    <row r="28" spans="1:10" ht="17.649999999999999" x14ac:dyDescent="0.45">
-      <c r="A28" s="47" t="s">
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="24"/>
+    </row>
+    <row r="30" spans="1:8" ht="17.649999999999999" x14ac:dyDescent="0.45">
+      <c r="A30" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="40"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="44"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="65"/>
-      <c r="J28" s="46"/>
-    </row>
-    <row r="29" spans="1:10" ht="17.649999999999999" x14ac:dyDescent="0.45">
-      <c r="A29" s="47" t="s">
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="24"/>
+    </row>
+    <row r="31" spans="1:8" ht="17.649999999999999" x14ac:dyDescent="0.45">
+      <c r="A31" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="42"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="65"/>
-      <c r="J29" s="46"/>
-    </row>
-    <row r="30" spans="1:10" ht="17.649999999999999" x14ac:dyDescent="0.45">
-      <c r="A30" s="47" t="s">
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="35"/>
+      <c r="H31" s="24"/>
+    </row>
+    <row r="32" spans="1:8" ht="17.649999999999999" x14ac:dyDescent="0.45">
+      <c r="A32" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="65"/>
-      <c r="J30" s="46"/>
-    </row>
-    <row r="31" spans="1:10" ht="17.649999999999999" x14ac:dyDescent="0.45">
-      <c r="A31" s="47" t="s">
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="24"/>
+    </row>
+    <row r="33" spans="1:8" ht="17.649999999999999" x14ac:dyDescent="0.45">
+      <c r="A33" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="44"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="65"/>
-      <c r="J31" s="46"/>
-    </row>
-    <row r="32" spans="1:10" ht="17.649999999999999" x14ac:dyDescent="0.45">
-      <c r="A32" s="47" t="s">
-        <v>14</v>
-      </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="42"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="44"/>
-      <c r="H32" s="45"/>
-      <c r="I32" s="65"/>
-      <c r="J32" s="46"/>
-    </row>
-    <row r="33" spans="1:10" ht="17.649999999999999" x14ac:dyDescent="0.45">
-      <c r="A33" s="47" t="s">
-        <v>15</v>
-      </c>
-      <c r="B33" s="40"/>
-      <c r="C33" s="40"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="42"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="44"/>
-      <c r="H33" s="45"/>
-      <c r="I33" s="65"/>
-      <c r="J33" s="46"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A25:J25"/>
-    <mergeCell ref="B26:J26"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="A25:H25"/>
+    <mergeCell ref="B26:H26"/>
     <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B3:F3"/>
     <mergeCell ref="B20:E20"/>
-    <mergeCell ref="A21:J21"/>
-    <mergeCell ref="A24:J24"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A24:H24"/>
     <mergeCell ref="B22:E22"/>
     <mergeCell ref="B23:E23"/>
     <mergeCell ref="A16:A18"/>
@@ -1850,18 +1724,6 @@
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B15:J15"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B11:J11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>